<commit_message>
Fix AZ-204 Develop event-based solutions section - removed 'Note: Creating event models is in scope' line
</commit_message>
<xml_diff>
--- a/Assessments/Exam-Msft-AZ-204-Self-Assessment-Build5Nines.xlsx
+++ b/Assessments/Exam-Msft-AZ-204-Self-Assessment-Build5Nines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e65a71525769dffd/Documenti/Penna Matteo/Azure Certification/AZ-204 Azure Certification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{3CCD204D-E6B6-4009-8EDC-BE517205B885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{51FA49EC-C8FE-4E29-9AE7-9A804FC8933C}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{3CCD204D-E6B6-4009-8EDC-BE517205B885}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2C7CFA8A-D465-4651-9F0F-E9AA0C543235}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="99">
   <si>
     <t>Microsoft Certification Self-Assessment Tool</t>
   </si>
@@ -317,12 +317,6 @@
     <t>define policies for APIs</t>
   </si>
   <si>
-    <t>Develop event-based solutions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Note: Creating event models is in scope </t>
-  </si>
-  <si>
     <t xml:space="preserve">implement solutions that use Azure Event Grid </t>
   </si>
   <si>
@@ -339,6 +333,9 @@
   </si>
   <si>
     <t>implement solutions that use Azure Queue Storage queues</t>
+  </si>
+  <si>
+    <t>Develop event-based solutions (Note: Creating event models is in scope)</t>
   </si>
 </sst>
 </file>
@@ -549,1174 +546,724 @@
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="156">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+  <dxfs count="111">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2581,49 +2128,49 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B16:B18 B20">
-    <cfRule type="cellIs" dxfId="155" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="9" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B18 B20">
-    <cfRule type="cellIs" dxfId="154" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="8" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B18 B20">
-    <cfRule type="cellIs" dxfId="153" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="108" priority="7" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="152" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="6" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="151" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="5" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21">
-    <cfRule type="cellIs" dxfId="150" priority="4" operator="between">
+    <cfRule type="cellIs" dxfId="105" priority="4" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="149" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="3" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="148" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="2" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B19">
-    <cfRule type="cellIs" dxfId="147" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="102" priority="1" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
@@ -2642,7 +2189,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
@@ -3072,7 +2619,7 @@
         <v>41</v>
       </c>
       <c r="D50" s="11">
-        <f>SUM(D51:D66)/4</f>
+        <f>SUM(D51:D65)/4</f>
         <v>0</v>
       </c>
     </row>
@@ -3144,16 +2691,16 @@
     </row>
     <row r="59" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B59" s="7" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D59" s="8">
-        <f>(VLOOKUP(D60,List_Categories,2,FALSE)+VLOOKUP(D61,List_Categories,2,FALSE)+VLOOKUP(D62,List_Categories,2,FALSE)+VLOOKUP(D63,List_Categories,2,FALSE))/4</f>
+        <f>(VLOOKUP(D60,List_Categories,2,FALSE)+VLOOKUP(D61,List_Categories,2,FALSE)++VLOOKUP(D62,List_Categories,2,FALSE))/3</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D60" t="s">
         <v>28</v>
@@ -3161,7 +2708,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D61" t="s">
         <v>28</v>
@@ -3169,430 +2716,407 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
+        <v>94</v>
+      </c>
+      <c r="D62" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B63" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="D62" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
+      <c r="D63" s="8">
+        <f>(VLOOKUP(D64,List_Categories,2,FALSE)+VLOOKUP(D65,List_Categories,2,FALSE))/2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
         <v>96</v>
       </c>
-      <c r="D63" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B64" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D64" s="8">
-        <f>(VLOOKUP(D65,List_Categories,2,FALSE)+VLOOKUP(D66,List_Categories,2,FALSE))/2</f>
-        <v>0</v>
+      <c r="D64" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C65" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D65" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>99</v>
-      </c>
-      <c r="D66" t="s">
-        <v>28</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="146" priority="278" operator="equal">
+  <conditionalFormatting sqref="D6 D60:D62">
+    <cfRule type="cellIs" dxfId="101" priority="278" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="145" priority="277" operator="equal">
+  <conditionalFormatting sqref="D6 D60:D62">
+    <cfRule type="cellIs" dxfId="100" priority="277" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="cellIs" dxfId="144" priority="276" operator="equal">
+  <conditionalFormatting sqref="D6 D60:D62">
+    <cfRule type="cellIs" dxfId="99" priority="276" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8">
-    <cfRule type="cellIs" dxfId="143" priority="275" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="275" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8">
-    <cfRule type="cellIs" dxfId="142" priority="274" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="274" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7:D8">
-    <cfRule type="cellIs" dxfId="141" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="273" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14">
-    <cfRule type="cellIs" dxfId="140" priority="272" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="272" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14">
-    <cfRule type="cellIs" dxfId="139" priority="271" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="271" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10:D14">
-    <cfRule type="cellIs" dxfId="138" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="270" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D18">
-    <cfRule type="cellIs" dxfId="137" priority="269" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="269" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D18">
-    <cfRule type="cellIs" dxfId="136" priority="268" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="268" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D18">
-    <cfRule type="cellIs" dxfId="135" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="267" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="131" priority="263" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="263" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="130" priority="262" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="262" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D21:D25">
-    <cfRule type="cellIs" dxfId="129" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="261" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D30">
-    <cfRule type="cellIs" dxfId="128" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="260" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D30">
-    <cfRule type="cellIs" dxfId="127" priority="259" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="259" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D30">
-    <cfRule type="cellIs" dxfId="126" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="258" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56:D58">
-    <cfRule type="cellIs" dxfId="119" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="215" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56:D58">
-    <cfRule type="cellIs" dxfId="118" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="214" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D56:D58">
-    <cfRule type="cellIs" dxfId="117" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="213" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D39">
-    <cfRule type="cellIs" dxfId="116" priority="248" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="248" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D39">
-    <cfRule type="cellIs" dxfId="115" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="247" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D37:D39">
-    <cfRule type="cellIs" dxfId="114" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="246" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:D54">
-    <cfRule type="cellIs" dxfId="113" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="218" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:D54">
-    <cfRule type="cellIs" dxfId="112" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="217" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D52:D54">
-    <cfRule type="cellIs" dxfId="111" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="216" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D63">
-    <cfRule type="cellIs" dxfId="110" priority="212" operator="equal">
+  <conditionalFormatting sqref="D64">
+    <cfRule type="cellIs" dxfId="74" priority="209" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D63">
-    <cfRule type="cellIs" dxfId="109" priority="211" operator="equal">
+  <conditionalFormatting sqref="D64">
+    <cfRule type="cellIs" dxfId="73" priority="208" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D60:D63">
-    <cfRule type="cellIs" dxfId="108" priority="210" operator="equal">
+  <conditionalFormatting sqref="D64">
+    <cfRule type="cellIs" dxfId="72" priority="207" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="107" priority="209" operator="equal">
-      <formula>"No Idea"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="106" priority="208" operator="equal">
-      <formula>"Know a Little"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D65">
-    <cfRule type="cellIs" dxfId="105" priority="207" operator="equal">
-      <formula>"Know Well"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="104" priority="189" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="189" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="103" priority="188" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="188" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="cellIs" dxfId="102" priority="187" operator="between">
+    <cfRule type="cellIs" dxfId="69" priority="187" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="101" priority="117" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="68" priority="117" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="100" priority="116" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="116" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="99" priority="115" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="115" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="98" priority="120" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="120" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="97" priority="119" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="119" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="cellIs" dxfId="96" priority="118" operator="between">
+    <cfRule type="cellIs" dxfId="63" priority="118" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="cellIs" dxfId="95" priority="114" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="62" priority="114" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="cellIs" dxfId="94" priority="113" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="113" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D31">
-    <cfRule type="cellIs" dxfId="93" priority="112" operator="between">
+    <cfRule type="cellIs" dxfId="60" priority="112" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="92" priority="111" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="111" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="91" priority="110" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="110" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D40">
-    <cfRule type="cellIs" dxfId="90" priority="109" operator="between">
+    <cfRule type="cellIs" dxfId="57" priority="109" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="89" priority="108" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="56" priority="108" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="88" priority="107" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="107" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D50">
-    <cfRule type="cellIs" dxfId="87" priority="106" operator="between">
+    <cfRule type="cellIs" dxfId="54" priority="106" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="86" priority="105" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="105" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="85" priority="104" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="104" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D9">
-    <cfRule type="cellIs" dxfId="84" priority="103" operator="between">
+    <cfRule type="cellIs" dxfId="51" priority="103" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="83" priority="102" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="102" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="82" priority="101" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="101" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="81" priority="100" operator="between">
+    <cfRule type="cellIs" dxfId="48" priority="100" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="62" priority="66" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="66" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="61" priority="65" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="65" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D26">
-    <cfRule type="cellIs" dxfId="60" priority="64" operator="between">
+    <cfRule type="cellIs" dxfId="45" priority="64" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="50" priority="69" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="69" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="49" priority="68" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="68" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D20">
-    <cfRule type="cellIs" dxfId="48" priority="67" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="67" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="44" priority="42" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="43" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D36">
-    <cfRule type="cellIs" dxfId="42" priority="40" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="cellIs" dxfId="41" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="27" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="cellIs" dxfId="40" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="26" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D51">
-    <cfRule type="cellIs" dxfId="39" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="25" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="cellIs" dxfId="38" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="24" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="cellIs" dxfId="37" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="23" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55">
-    <cfRule type="cellIs" dxfId="36" priority="22" operator="between">
-      <formula>0.5</formula>
-      <formula>0.7</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+    <cfRule type="cellIs" dxfId="33" priority="22" operator="between">
+      <formula>0.5</formula>
+      <formula>0.7</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D63">
     <cfRule type="cellIs" dxfId="32" priority="12" operator="greaterThan">
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="D63">
     <cfRule type="cellIs" dxfId="31" priority="11" operator="lessThan">
       <formula>0.5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D64">
+  <conditionalFormatting sqref="D63">
     <cfRule type="cellIs" dxfId="30" priority="10" operator="between">
       <formula>0.5</formula>
       <formula>0.7</formula>
@@ -3707,17 +3231,17 @@
       <formula>0.7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
+  <conditionalFormatting sqref="D65">
     <cfRule type="cellIs" dxfId="8" priority="15" operator="equal">
       <formula>"No Idea"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
+  <conditionalFormatting sqref="D65">
     <cfRule type="cellIs" dxfId="7" priority="14" operator="equal">
       <formula>"Know a Little"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D66">
+  <conditionalFormatting sqref="D65">
     <cfRule type="cellIs" dxfId="6" priority="13" operator="equal">
       <formula>"Know Well"</formula>
     </cfRule>
@@ -3761,7 +3285,7 @@
           <x14:formula1>
             <xm:f>'Other Values'!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D4:D8 D65:D66 D10:D14 D16:D18 D46:D49 D21:D25 D27:D30 D37:D39 D33:D35 D42:D44 D52:D54 D56:D58 D60:D63</xm:sqref>
+          <xm:sqref>D4:D8 D64:D65 D10:D14 D16:D18 D46:D49 D21:D25 D27:D30 D37:D39 D33:D35 D42:D44 D52:D54 D56:D58 D60:D62</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>